<commit_message>
CA Book 20220817 - Chapter 2
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8836354B-7488-4ECA-9DB1-F826232A7AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3C8D91-3651-4792-A037-E5B8BB0A84E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16530" yWindow="1365" windowWidth="20505" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23955" yWindow="1260" windowWidth="15270" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="181">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -739,6 +739,18 @@
   </si>
   <si>
     <t>등각성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>smooth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>매끄러운</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용어사전</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1064,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1790,6 +1802,17 @@
         <v>177</v>
       </c>
     </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>178</v>
+      </c>
+      <c r="B81" t="s">
+        <v>179</v>
+      </c>
+      <c r="D81" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D58" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D58">

</xml_diff>

<commit_message>
chapter 4 - working...
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\salt_data\MyWork_2022\MyPaper_2022\CA_Book_020221214\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD1CA6F-9D57-4700-B3F8-252CB298BE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A27B371-69D7-4DA3-A245-1856DF00BEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19365" yWindow="960" windowWidth="18375" windowHeight="14250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="213">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -855,6 +855,30 @@
   </si>
   <si>
     <t>상반평면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>supremum</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상계</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제곱급수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>complex power series</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>복소제곱급수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>띄어쓰기는?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1180,21 +1204,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="29.25" customWidth="1"/>
+    <col min="1" max="1" width="29.19921875" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" customWidth="1"/>
-    <col min="4" max="4" width="51.25" customWidth="1"/>
+    <col min="3" max="3" width="27.3984375" customWidth="1"/>
+    <col min="4" max="4" width="51.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1208,7 +1232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -1216,7 +1240,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -1224,7 +1248,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -1235,7 +1259,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -1249,7 +1273,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1260,7 +1284,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1268,7 +1292,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -1276,7 +1300,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1284,7 +1308,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>92</v>
       </c>
@@ -1292,7 +1316,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -1300,7 +1324,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1308,7 +1332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>151</v>
       </c>
@@ -1319,7 +1343,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1327,7 +1351,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -1335,7 +1359,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -1343,7 +1367,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1351,7 +1375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>175</v>
       </c>
@@ -1359,7 +1383,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1367,7 +1391,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -1381,7 +1405,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>180</v>
       </c>
@@ -1392,7 +1416,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -1403,7 +1427,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>182</v>
       </c>
@@ -1414,7 +1438,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1422,7 +1446,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>68</v>
       </c>
@@ -1430,7 +1454,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1452,7 +1476,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>144</v>
       </c>
@@ -1463,7 +1487,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -1474,7 +1498,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1482,7 +1506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -1490,7 +1514,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -1498,7 +1522,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>84</v>
       </c>
@@ -1506,7 +1530,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>126</v>
       </c>
@@ -1520,7 +1544,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>184</v>
       </c>
@@ -1528,7 +1552,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>157</v>
       </c>
@@ -1539,7 +1563,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>147</v>
       </c>
@@ -1547,7 +1571,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>167</v>
       </c>
@@ -1558,7 +1582,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -1566,7 +1590,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>110</v>
       </c>
@@ -1574,7 +1598,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1582,7 +1606,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>108</v>
       </c>
@@ -1590,7 +1614,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -1598,7 +1622,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>56</v>
       </c>
@@ -1606,7 +1630,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -1614,7 +1638,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>72</v>
       </c>
@@ -1622,7 +1646,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -1630,7 +1654,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>88</v>
       </c>
@@ -1638,7 +1662,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>100</v>
       </c>
@@ -1646,7 +1670,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>102</v>
       </c>
@@ -1654,7 +1678,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -1662,7 +1686,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>141</v>
       </c>
@@ -1673,7 +1697,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -1684,7 +1708,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -1692,7 +1716,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>62</v>
       </c>
@@ -1700,7 +1724,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>130</v>
       </c>
@@ -1708,7 +1732,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>74</v>
       </c>
@@ -1719,7 +1743,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>136</v>
       </c>
@@ -1730,7 +1754,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>106</v>
       </c>
@@ -1738,7 +1762,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -1746,7 +1770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>116</v>
       </c>
@@ -1757,15 +1781,21 @@
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>34</v>
       </c>
       <c r="B62" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>209</v>
+      </c>
+      <c r="D62" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>122</v>
       </c>
@@ -1773,7 +1803,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -1781,7 +1811,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>172</v>
       </c>
@@ -1792,7 +1822,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>161</v>
       </c>
@@ -1803,7 +1833,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>165</v>
       </c>
@@ -1811,7 +1841,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>54</v>
       </c>
@@ -1819,7 +1849,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -1827,7 +1857,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>163</v>
       </c>
@@ -1835,7 +1865,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>60</v>
       </c>
@@ -1843,7 +1873,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>58</v>
       </c>
@@ -1851,7 +1881,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -1859,7 +1889,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -1867,7 +1897,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -1875,7 +1905,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>32</v>
       </c>
@@ -1883,7 +1913,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>24</v>
       </c>
@@ -1891,7 +1921,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>10</v>
       </c>
@@ -1899,7 +1929,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -1907,7 +1937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>94</v>
       </c>
@@ -1915,7 +1945,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>177</v>
       </c>
@@ -1926,7 +1956,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -1934,7 +1964,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>104</v>
       </c>
@@ -1942,7 +1972,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>50</v>
       </c>
@@ -1950,7 +1980,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>187</v>
       </c>
@@ -1961,7 +1991,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>190</v>
       </c>
@@ -1975,7 +2005,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>193</v>
       </c>
@@ -1989,7 +2019,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>196</v>
       </c>
@@ -2000,7 +2030,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>198</v>
       </c>
@@ -2008,7 +2038,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>200</v>
       </c>
@@ -2019,7 +2049,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>202</v>
       </c>
@@ -2033,7 +2063,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>205</v>
       </c>
@@ -2042,6 +2072,28 @@
       </c>
       <c r="D92" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
+        <v>207</v>
+      </c>
+      <c r="B93" t="s">
+        <v>208</v>
+      </c>
+      <c r="D93" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
+        <v>210</v>
+      </c>
+      <c r="B94" t="s">
+        <v>211</v>
+      </c>
+      <c r="D94" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chapter 4 ... still..
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\salt_data\MyWork_2022\MyPaper_2022\CA_Book_020221214\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A27B371-69D7-4DA3-A245-1856DF00BEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578677BE-0414-42AC-8E86-BA5A33E0675D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13845" yWindow="3165" windowWidth="24090" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1206,19 +1206,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.19921875" customWidth="1"/>
+    <col min="1" max="1" width="29.25" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.3984375" customWidth="1"/>
-    <col min="4" max="4" width="51.19921875" customWidth="1"/>
+    <col min="3" max="3" width="27.375" customWidth="1"/>
+    <col min="4" max="4" width="51.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>114</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>96</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>92</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>151</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1351,754 +1351,754 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>78</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>175</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>42</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>132</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>133</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>134</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>180</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>181</v>
-      </c>
-      <c r="D21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>182</v>
-      </c>
-      <c r="B23" t="s">
-        <v>183</v>
       </c>
       <c r="D23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>18</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>68</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>8</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>124</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>144</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>139</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D31" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>202</v>
+      </c>
+      <c r="B32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" t="s">
+        <v>204</v>
+      </c>
+      <c r="D32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>138</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B33" t="s">
         <v>145</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D33" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>14</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>83</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B36" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>84</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>126</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B38" t="s">
         <v>127</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C38" t="s">
         <v>128</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D38" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>184</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B39" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>157</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B40" t="s">
         <v>158</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D40" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>147</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B41" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>193</v>
+      </c>
+      <c r="B42" t="s">
+        <v>194</v>
+      </c>
+      <c r="C42" t="s">
+        <v>195</v>
+      </c>
+      <c r="D42" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>167</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B43" t="s">
         <v>168</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D43" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>149</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B44" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>110</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B45" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>80</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B46" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>108</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B47" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>22</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B48" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>56</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B49" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>52</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B50" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>72</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B51" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>30</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B52" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>88</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B53" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>100</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B54" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>102</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B55" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>36</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B56" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>141</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B57" t="s">
         <v>142</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D57" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>170</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B58" t="s">
         <v>171</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D58" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>64</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B59" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>62</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B60" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>187</v>
+      </c>
+      <c r="B61" t="s">
+        <v>188</v>
+      </c>
+      <c r="D61" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>130</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B62" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>74</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B63" t="s">
         <v>75</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D63" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>136</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B64" t="s">
         <v>137</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D64" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>106</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B65" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>4</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B66" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>116</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B67" t="s">
         <v>117</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D67" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>34</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B68" t="s">
         <v>35</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C68" t="s">
         <v>209</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D68" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>122</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B69" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>86</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B70" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>172</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B71" t="s">
         <v>173</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C71" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A66" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>198</v>
+      </c>
+      <c r="B72" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>161</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B73" t="s">
         <v>162</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D73" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>165</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B74" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A68" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>54</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B75" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>48</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B76" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A70" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>163</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B77" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A71" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>60</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B78" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>58</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B79" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>70</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B80" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A74" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>28</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B81" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A75" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>26</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B82" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>32</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B83" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A77" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>24</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B84" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A78" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>10</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B85" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A79" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>7</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B86" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A80" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>94</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B87" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>177</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B88" t="s">
         <v>178</v>
-      </c>
-      <c r="D81" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
-        <v>160</v>
-      </c>
-      <c r="B82" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A83" t="s">
-        <v>104</v>
-      </c>
-      <c r="B83" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A84" t="s">
-        <v>50</v>
-      </c>
-      <c r="B84" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A85" t="s">
-        <v>187</v>
-      </c>
-      <c r="B85" t="s">
-        <v>188</v>
-      </c>
-      <c r="D85" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A86" t="s">
-        <v>190</v>
-      </c>
-      <c r="B86" t="s">
-        <v>191</v>
-      </c>
-      <c r="C86" t="s">
-        <v>192</v>
-      </c>
-      <c r="D86" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
-        <v>193</v>
-      </c>
-      <c r="B87" t="s">
-        <v>194</v>
-      </c>
-      <c r="C87" t="s">
-        <v>195</v>
-      </c>
-      <c r="D87" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
-        <v>196</v>
-      </c>
-      <c r="B88" t="s">
-        <v>197</v>
       </c>
       <c r="D88" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="B89" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>207</v>
+      </c>
+      <c r="B90" t="s">
+        <v>208</v>
+      </c>
+      <c r="D90" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>104</v>
+      </c>
+      <c r="B91" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>50</v>
+      </c>
+      <c r="B92" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>205</v>
+      </c>
+      <c r="B93" t="s">
+        <v>206</v>
+      </c>
+      <c r="D93" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>200</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B94" t="s">
         <v>201</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D94" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A91" t="s">
-        <v>202</v>
-      </c>
-      <c r="B91" t="s">
-        <v>203</v>
-      </c>
-      <c r="C91" t="s">
-        <v>204</v>
-      </c>
-      <c r="D91" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A92" t="s">
-        <v>205</v>
-      </c>
-      <c r="B92" t="s">
-        <v>206</v>
-      </c>
-      <c r="D92" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A93" t="s">
-        <v>207</v>
-      </c>
-      <c r="B93" t="s">
-        <v>208</v>
-      </c>
-      <c r="D93" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A94" t="s">
-        <v>210</v>
-      </c>
-      <c r="B94" t="s">
-        <v>211</v>
-      </c>
-      <c r="D94" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D58" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D84">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D94">
       <sortCondition ref="A1:A58"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
chapter 4 ... ing
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578677BE-0414-42AC-8E86-BA5A33E0675D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754DA84B-72D1-4B51-BA73-2636E6E01322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13845" yWindow="3165" windowWidth="24090" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="221">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -879,6 +879,38 @@
   </si>
   <si>
     <t>띄어쓰기는?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>multiplicity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중복도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근의 차수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zero</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근으로 통일 (해보다는…)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1204,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2096,6 +2128,39 @@
         <v>179</v>
       </c>
     </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>213</v>
+      </c>
+      <c r="B95" t="s">
+        <v>214</v>
+      </c>
+      <c r="D95" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>215</v>
+      </c>
+      <c r="B96" t="s">
+        <v>216</v>
+      </c>
+      <c r="D96" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>218</v>
+      </c>
+      <c r="B97" t="s">
+        <v>219</v>
+      </c>
+      <c r="D97" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D58" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D94">

</xml_diff>

<commit_message>
Chapter 4 - Laurent series done!
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1495087-C71E-44D3-881F-971D9CC320E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D33A05C-D29A-4A21-A4C1-3A36236AF76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13845" yWindow="3165" windowWidth="24090" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="230">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -542,14 +542,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>복소해석</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>복소해석으로 통일함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>path-connected</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -919,6 +911,42 @@
   </si>
   <si>
     <t xml:space="preserve">정역 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>removable singularity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제거가능한 특이점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>essential singularity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>본질적 특이점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>복소해석, 해석적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>복소해석으로 통일함 형용사로 해석적 (서울대 교재 참고)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Casorati</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카소라티</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>임의로 번역</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1244,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D98"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1301,16 +1329,16 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" t="s">
         <v>154</v>
       </c>
-      <c r="B5" t="s">
-        <v>155</v>
-      </c>
-      <c r="C5" t="s">
-        <v>156</v>
-      </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1374,13 +1402,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1393,13 +1421,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>207</v>
+      </c>
+      <c r="B15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" t="s">
         <v>209</v>
-      </c>
-      <c r="B15" t="s">
-        <v>210</v>
-      </c>
-      <c r="D15" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1412,16 +1440,16 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" t="s">
         <v>190</v>
       </c>
-      <c r="B17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" t="s">
-        <v>192</v>
-      </c>
       <c r="D17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1442,10 +1470,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1458,38 +1486,38 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" t="s">
         <v>132</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>133</v>
-      </c>
-      <c r="C22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D22" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1500,18 +1528,18 @@
         <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1554,38 +1582,38 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" t="s">
         <v>144</v>
-      </c>
-      <c r="B31" t="s">
-        <v>139</v>
-      </c>
-      <c r="D31" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>200</v>
+      </c>
+      <c r="B32" t="s">
+        <v>201</v>
+      </c>
+      <c r="C32" t="s">
         <v>202</v>
       </c>
-      <c r="B32" t="s">
-        <v>203</v>
-      </c>
-      <c r="C32" t="s">
-        <v>204</v>
-      </c>
       <c r="D32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D33" t="s">
         <v>138</v>
-      </c>
-      <c r="B33" t="s">
-        <v>145</v>
-      </c>
-      <c r="D33" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1628,70 +1656,70 @@
         <v>127</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>225</v>
       </c>
       <c r="D38" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B39" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>191</v>
+      </c>
+      <c r="B42" t="s">
+        <v>192</v>
+      </c>
+      <c r="C42" t="s">
         <v>193</v>
       </c>
-      <c r="B42" t="s">
-        <v>194</v>
-      </c>
-      <c r="C42" t="s">
-        <v>195</v>
-      </c>
       <c r="D42" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="s">
         <v>167</v>
-      </c>
-      <c r="B43" t="s">
-        <v>168</v>
-      </c>
-      <c r="D43" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1792,24 +1820,24 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>139</v>
+      </c>
+      <c r="B57" t="s">
+        <v>140</v>
+      </c>
+      <c r="D57" t="s">
         <v>141</v>
-      </c>
-      <c r="B57" t="s">
-        <v>142</v>
-      </c>
-      <c r="D57" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B58" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D58" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1830,21 +1858,21 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" t="s">
+        <v>186</v>
+      </c>
+      <c r="D61" t="s">
         <v>187</v>
-      </c>
-      <c r="B61" t="s">
-        <v>188</v>
-      </c>
-      <c r="D61" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B62" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1860,13 +1888,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D64" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1904,10 +1932,10 @@
         <v>35</v>
       </c>
       <c r="C68" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D68" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,40 +1956,40 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>170</v>
+      </c>
+      <c r="B71" t="s">
+        <v>171</v>
+      </c>
+      <c r="C71" t="s">
         <v>172</v>
-      </c>
-      <c r="B71" t="s">
-        <v>173</v>
-      </c>
-      <c r="C71" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B72" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B73" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D73" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B74" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1982,10 +2010,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B77" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2070,29 +2098,29 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>175</v>
+      </c>
+      <c r="B88" t="s">
+        <v>176</v>
+      </c>
+      <c r="D88" t="s">
         <v>177</v>
-      </c>
-      <c r="B88" t="s">
-        <v>178</v>
-      </c>
-      <c r="D88" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B89" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B90" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D90" t="s">
         <v>121</v>
@@ -2116,68 +2144,98 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B93" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D93" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B94" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D94" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B95" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D95" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>212</v>
+      </c>
+      <c r="B96" t="s">
+        <v>213</v>
+      </c>
+      <c r="D96" t="s">
         <v>214</v>
-      </c>
-      <c r="B96" t="s">
-        <v>215</v>
-      </c>
-      <c r="D96" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>215</v>
+      </c>
+      <c r="B97" t="s">
+        <v>216</v>
+      </c>
+      <c r="D97" t="s">
         <v>217</v>
-      </c>
-      <c r="B97" t="s">
-        <v>218</v>
-      </c>
-      <c r="D97" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
+        <v>219</v>
+      </c>
+      <c r="B98" t="s">
+        <v>220</v>
+      </c>
+      <c r="D98" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>221</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>222</v>
       </c>
-      <c r="D98" t="s">
-        <v>179</v>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>223</v>
+      </c>
+      <c r="B100" t="s">
+        <v>224</v>
+      </c>
+      <c r="D100" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>227</v>
+      </c>
+      <c r="B101" t="s">
+        <v>228</v>
+      </c>
+      <c r="D101" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chapter 5 - ing
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D33A05C-D29A-4A21-A4C1-3A36236AF76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6923F4-0B27-4BBA-9466-2F3207EA27CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13845" yWindow="3165" windowWidth="24090" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11355" yWindow="2115" windowWidth="24090" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$58</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="234">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -947,6 +958,22 @@
   </si>
   <si>
     <t>임의로 번역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fundamental theorem of integral calculus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적분학의 기본정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>maximum principle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최대원리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1272,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2238,6 +2265,28 @@
         <v>229</v>
       </c>
     </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>230</v>
+      </c>
+      <c r="B102" t="s">
+        <v>231</v>
+      </c>
+      <c r="D102" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>232</v>
+      </c>
+      <c r="B103" t="s">
+        <v>233</v>
+      </c>
+      <c r="D103" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D58" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D94">

</xml_diff>

<commit_message>
Sol - chapter 3- end, ch4 -ing
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6923F4-0B27-4BBA-9466-2F3207EA27CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580ED7CE-818C-4892-9B9E-C9E7A80667F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11355" yWindow="2115" windowWidth="24090" windowHeight="12090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12735" yWindow="1050" windowWidth="24090" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="236">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -974,6 +974,14 @@
   </si>
   <si>
     <t>최대원리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근판정법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근판정법(용어사전)으로 통일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1301,8 +1309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2090,6 +2098,12 @@
       <c r="B83" t="s">
         <v>33</v>
       </c>
+      <c r="C83" t="s">
+        <v>234</v>
+      </c>
+      <c r="D83" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">

</xml_diff>

<commit_message>
draft 5 - chapter 1 - ing
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580ED7CE-818C-4892-9B9E-C9E7A80667F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D543F3DF-0004-4356-AC28-817797C56FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12735" yWindow="1050" windowWidth="24090" windowHeight="14265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11880" yWindow="1020" windowWidth="25770" windowHeight="12825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="번역" sheetId="1" r:id="rId1"/>
+    <sheet name="용어통일" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">번역!$A$1:$D$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="241">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -982,6 +983,26 @@
   </si>
   <si>
     <t>근판정법(용어사전)으로 통일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>복소미분가능 함수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코시 적분정리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경로연결 집합, 열린 경로연결 집합</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x-축</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우측 반평면, 좌측 반평면, 상반평면, 하반평면</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1309,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2311,4 +2332,49 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759B79D5-F890-47B4-8854-6B46C939DF26}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="67.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
draft  5 - chapter 2 - ing - p66
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D543F3DF-0004-4356-AC28-817797C56FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA91A38-C831-4FA8-AE6B-3C78541430D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11880" yWindow="1020" windowWidth="25770" windowHeight="12825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="245">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1003,6 +1003,22 @@
   </si>
   <si>
     <t>우측 반평면, 좌측 반평면, 상반평면, 하반평면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>열린 집합, 닫힌 집합</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>entire function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전해석 함수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뚫린원판</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1328,10 +1344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D104"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2319,6 +2335,17 @@
         <v>233</v>
       </c>
       <c r="D103" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>242</v>
+      </c>
+      <c r="B104" t="s">
+        <v>243</v>
+      </c>
+      <c r="D104" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2336,10 +2363,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759B79D5-F890-47B4-8854-6B46C939DF26}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2372,6 +2399,16 @@
         <v>240</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>244</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
draft 5 - chapter 2 - end
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA91A38-C831-4FA8-AE6B-3C78541430D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F66FAF6-4D3C-428C-B532-7FB3938F70E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="1020" windowWidth="25770" windowHeight="12825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11880" yWindow="1020" windowWidth="25770" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="번역" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="247">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -986,10 +986,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>복소미분가능 함수</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>코시 적분정리</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1019,6 +1015,18 @@
   </si>
   <si>
     <t>뚫린원판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미분가능 함수, 복소미분가능 함수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>differential operator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미분 작용소</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1344,10 +1352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D104"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2340,12 +2348,23 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>241</v>
+      </c>
+      <c r="B104" t="s">
         <v>242</v>
       </c>
-      <c r="B104" t="s">
-        <v>243</v>
-      </c>
       <c r="D104" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>245</v>
+      </c>
+      <c r="B105" t="s">
+        <v>246</v>
+      </c>
+      <c r="D105" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2365,9 +2384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759B79D5-F890-47B4-8854-6B46C939DF26}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2376,37 +2393,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draft 5 - chap3
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F66FAF6-4D3C-428C-B532-7FB3938F70E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCAB453-794F-4CD3-A41A-395742EC6133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="1020" windowWidth="25770" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11880" yWindow="1020" windowWidth="25770" windowHeight="12825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="번역" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="249">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1014,10 +1014,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>뚫린원판</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>미분가능 함수, 복소미분가능 함수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1027,6 +1023,18 @@
   </si>
   <si>
     <t>미분 작용소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적분값, 경로적분값</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리만 적분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뚫린 원판, 뚫린 평면</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1354,8 +1362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106"/>
+    <sheetView topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2359,10 +2367,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
+        <v>244</v>
+      </c>
+      <c r="B105" t="s">
         <v>245</v>
-      </c>
-      <c r="B105" t="s">
-        <v>246</v>
       </c>
       <c r="D105" t="s">
         <v>177</v>
@@ -2382,9 +2390,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759B79D5-F890-47B4-8854-6B46C939DF26}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2393,7 +2403,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -2423,7 +2433,17 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>243</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draft5 - chapter 4.5 (165p)
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCAB453-794F-4CD3-A41A-395742EC6133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6BAB75-5CCE-4CD6-927C-D890B98093E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11880" yWindow="1020" windowWidth="25770" windowHeight="12825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="255">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1035,6 +1035,30 @@
   </si>
   <si>
     <t>뚫린 원판, 뚫린 평면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테일러 급수, 로랑 급수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>근의 분류</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영점, 극점, 본질적 특이점, n차 극점, 단순 극점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수렴 반지름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수렴 반지름으로 통일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수렴 반지름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1363,7 +1387,7 @@
   <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2086,6 +2110,12 @@
       </c>
       <c r="B75" t="s">
         <v>55</v>
+      </c>
+      <c r="C75" t="s">
+        <v>252</v>
+      </c>
+      <c r="D75" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2390,10 +2420,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759B79D5-F890-47B4-8854-6B46C939DF26}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2446,6 +2476,26 @@
         <v>247</v>
       </c>
     </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>254</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
draft 5 - chapter 5 - ing
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6BAB75-5CCE-4CD6-927C-D890B98093E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB79D1F0-3332-4332-8197-79D6441EEC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11880" yWindow="1020" windowWidth="25770" windowHeight="12825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="258">
   <si>
     <t>영문 용어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,10 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>닫힌곡선</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Fundamental theorem of algebra</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -302,10 +298,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>열린원판</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>anti-derivative</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1059,6 +1051,26 @@
   </si>
   <si>
     <t>수렴 반지름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원형 경로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닫힌 곡선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>열린 원판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단순연결 영역</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단위 원판</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1386,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1414,94 +1426,94 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" t="s">
         <v>119</v>
-      </c>
-      <c r="B4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" t="s">
         <v>152</v>
       </c>
-      <c r="B5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C5" t="s">
-        <v>154</v>
-      </c>
       <c r="D5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1509,165 +1521,165 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" t="s">
         <v>207</v>
-      </c>
-      <c r="B15" t="s">
-        <v>208</v>
-      </c>
-      <c r="D15" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C17" t="s">
         <v>188</v>
       </c>
-      <c r="B17" t="s">
-        <v>189</v>
-      </c>
-      <c r="C17" t="s">
-        <v>190</v>
-      </c>
       <c r="D17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
         <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B20" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
         <v>42</v>
-      </c>
-      <c r="B21" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" t="s">
         <v>130</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>131</v>
-      </c>
-      <c r="C22" t="s">
-        <v>132</v>
-      </c>
-      <c r="D22" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" t="s">
         <v>44</v>
       </c>
-      <c r="B25" t="s">
-        <v>45</v>
-      </c>
       <c r="D25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
         <v>18</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1686,335 +1698,335 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" t="s">
         <v>142</v>
-      </c>
-      <c r="B31" t="s">
-        <v>137</v>
-      </c>
-      <c r="D31" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" t="s">
         <v>200</v>
       </c>
-      <c r="B32" t="s">
-        <v>201</v>
-      </c>
-      <c r="C32" t="s">
-        <v>202</v>
-      </c>
       <c r="D32" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" t="s">
+        <v>141</v>
+      </c>
+      <c r="D33" t="s">
         <v>136</v>
-      </c>
-      <c r="B33" t="s">
-        <v>143</v>
-      </c>
-      <c r="D33" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" t="s">
         <v>14</v>
-      </c>
-      <c r="B34" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" t="s">
         <v>38</v>
-      </c>
-      <c r="B35" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C38" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D38" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B41" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>189</v>
+      </c>
+      <c r="B42" t="s">
+        <v>190</v>
+      </c>
+      <c r="C42" t="s">
         <v>191</v>
       </c>
-      <c r="B42" t="s">
-        <v>192</v>
-      </c>
-      <c r="C42" t="s">
-        <v>193</v>
-      </c>
       <c r="D42" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" t="s">
         <v>165</v>
-      </c>
-      <c r="B43" t="s">
-        <v>166</v>
-      </c>
-      <c r="D43" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" t="s">
         <v>22</v>
-      </c>
-      <c r="B48" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" t="s">
         <v>56</v>
-      </c>
-      <c r="B49" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
         <v>52</v>
-      </c>
-      <c r="B50" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" t="s">
         <v>30</v>
-      </c>
-      <c r="B52" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B54" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" t="s">
         <v>36</v>
-      </c>
-      <c r="B56" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>137</v>
+      </c>
+      <c r="B57" t="s">
+        <v>138</v>
+      </c>
+      <c r="D57" t="s">
         <v>139</v>
-      </c>
-      <c r="B57" t="s">
-        <v>140</v>
-      </c>
-      <c r="D57" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B58" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D58" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>255</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" t="s">
         <v>62</v>
-      </c>
-      <c r="B60" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>183</v>
+      </c>
+      <c r="B61" t="s">
+        <v>184</v>
+      </c>
+      <c r="D61" t="s">
         <v>185</v>
-      </c>
-      <c r="B61" t="s">
-        <v>186</v>
-      </c>
-      <c r="D61" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" t="s">
+        <v>73</v>
+      </c>
+      <c r="D63" t="s">
         <v>74</v>
-      </c>
-      <c r="B63" t="s">
-        <v>75</v>
-      </c>
-      <c r="D63" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B64" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D64" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2027,173 +2039,173 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67" t="s">
+        <v>115</v>
+      </c>
+      <c r="D67" t="s">
         <v>116</v>
-      </c>
-      <c r="B67" t="s">
-        <v>117</v>
-      </c>
-      <c r="D67" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>33</v>
+      </c>
+      <c r="B68" t="s">
         <v>34</v>
       </c>
-      <c r="B68" t="s">
-        <v>35</v>
-      </c>
       <c r="C68" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D68" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B69" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>168</v>
+      </c>
+      <c r="B71" t="s">
+        <v>169</v>
+      </c>
+      <c r="C71" t="s">
         <v>170</v>
-      </c>
-      <c r="B71" t="s">
-        <v>171</v>
-      </c>
-      <c r="C71" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B72" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B73" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D73" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B74" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>53</v>
+      </c>
+      <c r="B75" t="s">
         <v>54</v>
       </c>
-      <c r="B75" t="s">
-        <v>55</v>
-      </c>
       <c r="C75" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76" t="s">
         <v>48</v>
-      </c>
-      <c r="B76" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B77" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>59</v>
+      </c>
+      <c r="B78" t="s">
         <v>60</v>
-      </c>
-      <c r="B78" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79" t="s">
         <v>58</v>
-      </c>
-      <c r="B79" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B80" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81" t="s">
         <v>28</v>
-      </c>
-      <c r="B81" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>25</v>
+      </c>
+      <c r="B82" t="s">
         <v>26</v>
-      </c>
-      <c r="B82" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83" t="s">
         <v>32</v>
       </c>
-      <c r="B83" t="s">
-        <v>33</v>
-      </c>
       <c r="C83" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D83" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" t="s">
         <v>24</v>
-      </c>
-      <c r="B84" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2214,196 +2226,196 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B87" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>173</v>
+      </c>
+      <c r="B88" t="s">
+        <v>174</v>
+      </c>
+      <c r="D88" t="s">
         <v>175</v>
-      </c>
-      <c r="B88" t="s">
-        <v>176</v>
-      </c>
-      <c r="D88" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B89" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B90" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D90" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B91" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>49</v>
+      </c>
+      <c r="B92" t="s">
         <v>50</v>
-      </c>
-      <c r="B92" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B93" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D93" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B94" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D94" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B95" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D95" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>210</v>
+      </c>
+      <c r="B96" t="s">
+        <v>211</v>
+      </c>
+      <c r="D96" t="s">
         <v>212</v>
-      </c>
-      <c r="B96" t="s">
-        <v>213</v>
-      </c>
-      <c r="D96" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>213</v>
+      </c>
+      <c r="B97" t="s">
+        <v>214</v>
+      </c>
+      <c r="D97" t="s">
         <v>215</v>
-      </c>
-      <c r="B97" t="s">
-        <v>216</v>
-      </c>
-      <c r="D97" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B98" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D98" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B99" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B100" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D100" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>225</v>
+      </c>
+      <c r="B101" t="s">
+        <v>226</v>
+      </c>
+      <c r="D101" t="s">
         <v>227</v>
-      </c>
-      <c r="B101" t="s">
-        <v>228</v>
-      </c>
-      <c r="D101" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B102" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D102" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B103" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D103" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B104" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D104" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B105" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D105" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -2420,10 +2432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759B79D5-F890-47B4-8854-6B46C939DF26}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2433,67 +2445,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>254</v>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dfaft 6 - indexing. Hur's comments -- ing
</commit_message>
<xml_diff>
--- a/word_list.xlsx
+++ b/word_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\salt_data\Git_2022\CA_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB79D1F0-3332-4332-8197-79D6441EEC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBBCC9A-448F-4A73-BE65-C757722A63F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="1020" windowWidth="25770" windowHeight="12825" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="25770" windowHeight="12825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="번역" sheetId="1" r:id="rId1"/>
@@ -1398,7 +1398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
@@ -2434,8 +2434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759B79D5-F890-47B4-8854-6B46C939DF26}">
   <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>